<commit_message>
Added to test plan doc
</commit_message>
<xml_diff>
--- a/documentation/TestPlan.xlsx
+++ b/documentation/TestPlan.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27715"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joecho/Documents/CS411/spotify-playlist-extender/documentation/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="9768" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="23260" windowHeight="9760" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Form Validation" sheetId="1" r:id="rId1"/>
@@ -12,12 +17,20 @@
     <sheet name="UI Validation" sheetId="3" r:id="rId3"/>
     <sheet name="Remediation" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="134">
   <si>
     <t>Page Name</t>
   </si>
@@ -371,6 +384,54 @@
   </si>
   <si>
     <t>ui.29</t>
+  </si>
+  <si>
+    <t>json</t>
+  </si>
+  <si>
+    <t>issues with calls to the mongo db not returning valid json</t>
+  </si>
+  <si>
+    <t>json1</t>
+  </si>
+  <si>
+    <t>ui2</t>
+  </si>
+  <si>
+    <t>ui3</t>
+  </si>
+  <si>
+    <t>field1</t>
+  </si>
+  <si>
+    <t>ui1</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>login via spotify does not display welcome message in correct place</t>
+  </si>
+  <si>
+    <t>Joe/Cullen</t>
+  </si>
+  <si>
+    <t>ui4</t>
+  </si>
+  <si>
+    <t>rsearches</t>
+  </si>
+  <si>
+    <t>recent search results not displaying in columns</t>
+  </si>
+  <si>
+    <t>mongo1</t>
+  </si>
+  <si>
+    <t>json2</t>
+  </si>
+  <si>
+    <t>index/home not property passing "similar tracks" to similar tracks page</t>
   </si>
 </sst>
 </file>
@@ -478,12 +539,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -513,12 +574,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -724,20 +785,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" customWidth="1"/>
-    <col min="2" max="2" width="29.5546875" customWidth="1"/>
+    <col min="1" max="1" width="11.5" customWidth="1"/>
+    <col min="2" max="2" width="29.5" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
     <col min="4" max="4" width="22.33203125" customWidth="1"/>
-    <col min="5" max="5" width="22.44140625" customWidth="1"/>
+    <col min="5" max="5" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -757,7 +818,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -777,7 +838,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -797,7 +858,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -817,7 +878,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -837,7 +898,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -857,7 +918,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -877,7 +938,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -897,7 +958,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -917,7 +978,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -950,16 +1011,16 @@
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" customWidth="1"/>
+    <col min="1" max="1" width="14.5" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" customWidth="1"/>
+    <col min="5" max="5" width="12.5" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="8" max="8" width="42.5546875" customWidth="1"/>
+    <col min="8" max="8" width="42.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -988,7 +1049,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -1017,7 +1078,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>43</v>
       </c>
@@ -1046,7 +1107,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -1075,7 +1136,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -1104,7 +1165,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -1133,7 +1194,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -1175,14 +1236,14 @@
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.21875" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" customWidth="1"/>
-    <col min="3" max="3" width="26.109375" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" customWidth="1"/>
+    <col min="3" max="3" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1199,7 +1260,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1216,7 +1277,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1233,7 +1294,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1250,7 +1311,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1267,7 +1328,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1284,7 +1345,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1301,7 +1362,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1318,7 +1379,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1335,7 +1396,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -1352,7 +1413,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -1369,7 +1430,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -1386,7 +1447,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -1403,7 +1464,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -1420,7 +1481,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -1437,7 +1498,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -1454,7 +1515,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -1471,7 +1532,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -1488,7 +1549,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -1505,7 +1566,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -1522,7 +1583,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -1539,7 +1600,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>5</v>
       </c>
@@ -1556,7 +1617,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>56</v>
       </c>
@@ -1573,7 +1634,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>56</v>
       </c>
@@ -1590,7 +1651,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>56</v>
       </c>
@@ -1607,7 +1668,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>56</v>
       </c>
@@ -1624,7 +1685,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>62</v>
       </c>
@@ -1641,7 +1702,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>62</v>
       </c>
@@ -1658,7 +1719,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>62</v>
       </c>
@@ -1675,7 +1736,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>62</v>
       </c>
@@ -1699,21 +1760,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="50.21875" customWidth="1"/>
-    <col min="4" max="4" width="12.21875" customWidth="1"/>
-    <col min="5" max="5" width="9.5546875" customWidth="1"/>
+    <col min="3" max="3" width="50.1640625" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" customWidth="1"/>
+    <col min="5" max="5" width="9.5" customWidth="1"/>
     <col min="6" max="6" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1733,9 +1794,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>123</v>
       </c>
       <c r="B2" t="s">
         <v>26</v>
@@ -1753,9 +1814,9 @@
         <v>42709</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>121</v>
       </c>
       <c r="B3" t="s">
         <v>58</v>
@@ -1773,9 +1834,9 @@
         <v>42709</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>122</v>
       </c>
       <c r="B4" t="s">
         <v>63</v>
@@ -1790,6 +1851,86 @@
         <v>60</v>
       </c>
       <c r="F4" s="1">
+        <v>42709</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>127</v>
+      </c>
+      <c r="F5" s="1">
+        <v>42709</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C6" t="s">
+        <v>126</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F6" s="1">
+        <v>42709</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>128</v>
+      </c>
+      <c r="B7" t="s">
+        <v>129</v>
+      </c>
+      <c r="C7" t="s">
+        <v>130</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7" s="1">
+        <v>42709</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B8" t="s">
+        <v>132</v>
+      </c>
+      <c r="C8" t="s">
+        <v>133</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="1">
         <v>42709</v>
       </c>
     </row>

</xml_diff>